<commit_message>
updated schedule and Android App
</commit_message>
<xml_diff>
--- a/07_Templates/03_ProductBurndown/schedule.xlsx
+++ b/07_Templates/03_ProductBurndown/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\alex\3. Klasse\syp\if.05.61_01-project-repository\07_Templates\03_ProductBurndown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexb\HTBLA_Leonding\3.Klasse\SYP\MTB-Tracker\07_Templates\03_ProductBurndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45CA088-66B7-4674-BBC4-764CD560A1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BFE60C-3FE8-4A56-8407-2F9C3F6E506A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Task</t>
   </si>
@@ -45,16 +45,31 @@
     <t>Responsible</t>
   </si>
   <si>
-    <t>Hardware Prototyp</t>
-  </si>
-  <si>
-    <t>Software App</t>
-  </si>
-  <si>
     <t>Software Testing</t>
   </si>
   <si>
     <t>Firmware Prototyp</t>
+  </si>
+  <si>
+    <t>Harware Selection</t>
+  </si>
+  <si>
+    <t>Hardware Assembly</t>
+  </si>
+  <si>
+    <t>Hardware Enclosure</t>
+  </si>
+  <si>
+    <t>Software Technology Selection</t>
+  </si>
+  <si>
+    <t>Software "Hello World"</t>
+  </si>
+  <si>
+    <t>Software Coding</t>
+  </si>
+  <si>
+    <t>Testing/Shredding</t>
   </si>
 </sst>
 </file>
@@ -372,18 +387,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,72 +419,157 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>20</v>
       </c>
-      <c r="C4">
+      <c r="C9">
         <v>20</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>